<commit_message>
Enhanced Dispatcher with attachment handling and queue updates
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thhllc-my.sharepoint.com/personal/moris_wachira_griffinglobaltech_com/Documents/Documents/UiPath/T2G_EmailAutomation/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thhllc-my.sharepoint.com/personal/moris_wachira_griffinglobaltech_com/Documents/Documents/UiPath/T2G_EmailEnricher/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE11B82-931B-4669-9967-632EA08F9A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{7FE11B82-931B-4669-9967-632EA08F9A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8B483D8-3C2F-41EC-89A2-02E73BE9F981}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="68">
   <si>
     <t>Name</t>
   </si>
@@ -236,6 +236,18 @@
 Let me know once it's fixed so I can retry.
 Best regards,  
 Robot :)</t>
+  </si>
+  <si>
+    <t>AttachmentsFolder</t>
+  </si>
+  <si>
+    <t>C:\Users\MorisMwaiWachira\OneDrive - THH LLC\Documents\UiPath\T2G_EmailEnricher\Data\Output\Attachments</t>
+  </si>
+  <si>
+    <t>ProcessedEmailsFolder</t>
+  </si>
+  <si>
+    <t>Processed Mails</t>
   </si>
 </sst>
 </file>
@@ -313,6 +325,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -614,7 +630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -705,10 +721,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z27"/>
+  <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -950,6 +966,22 @@
       </c>
       <c r="B27" s="3" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="45">
+      <c r="A29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update attachments folder relative path
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thhllc-my.sharepoint.com/personal/moris_wachira_griffinglobaltech_com/Documents/Documents/UiPath/T2G_EmailEnricher/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{7FE11B82-931B-4669-9967-632EA08F9A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8B483D8-3C2F-41EC-89A2-02E73BE9F981}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{7FE11B82-931B-4669-9967-632EA08F9A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8090B21F-B0FB-49B3-BA17-C3E8A3B3D55D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -160,9 +160,6 @@
   </si>
   <si>
     <t>ExcelReportPath</t>
-  </si>
-  <si>
-    <t>NotificationEmail</t>
   </si>
   <si>
     <t>FilteredEmailsQueue</t>
@@ -241,13 +238,22 @@
     <t>AttachmentsFolder</t>
   </si>
   <si>
-    <t>C:\Users\MorisMwaiWachira\OneDrive - THH LLC\Documents\UiPath\T2G_EmailEnricher\Data\Output\Attachments</t>
-  </si>
-  <si>
     <t>ProcessedEmailsFolder</t>
   </si>
   <si>
     <t>Processed Mails</t>
+  </si>
+  <si>
+    <t>Data\Output\Attachments</t>
+  </si>
+  <si>
+    <t>ProcessedAttachmentsFolder</t>
+  </si>
+  <si>
+    <t>ExceptionNotificationEmail</t>
+  </si>
+  <si>
+    <t>SummaryNotificationEmail</t>
   </si>
 </sst>
 </file>
@@ -681,7 +687,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -692,7 +698,7 @@
         <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>43</v>
@@ -723,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -906,82 +912,82 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="195">
       <c r="A24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="180">
       <c r="A25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="150">
       <c r="A26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="195">
       <c r="A27" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="3" t="s">
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="45">
-      <c r="A29" t="s">
-        <v>64</v>
-      </c>
       <c r="B29" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -994,7 +1000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1052,15 +1058,36 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Refactored Dispatcher to use List<MailMessage> as TransactionItem and removed Orchestrator transaction dependency
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thhllc-my.sharepoint.com/personal/moris_wachira_griffinglobaltech_com/Documents/Documents/UiPath/T2G_EmailEnricher/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\OneDrive - THH LLC\Documents\UiPath\T2G_EmailEnricher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{7FE11B82-931B-4669-9967-632EA08F9A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8090B21F-B0FB-49B3-BA17-C3E8A3B3D55D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1211CB50-1440-4854-8B3F-5896B67D3F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t>Automation error!</t>
-  </si>
-  <si>
-    <t>No emails found</t>
   </si>
   <si>
     <t>No Valid Attachment Found</t>
@@ -208,19 +205,6 @@
 Robot :)</t>
   </si>
   <si>
-    <t>BusinessExEmailSubject_NoEmailsFound</t>
-  </si>
-  <si>
-    <t>BusinessExEmailBody_NoEmailsFound</t>
-  </si>
-  <si>
-    <t>Hello,
-The automation did not find any emails matching the specified criteria within the last 7 days.
-If this seems unexpected, please confirm the filter phrases or email delivery.
-Best regards,  
-Robot :)</t>
-  </si>
-  <si>
     <t>BusinessExEmailSubject_InvalidExcelFormat</t>
   </si>
   <si>
@@ -254,6 +238,38 @@
   </si>
   <si>
     <t>SummaryNotificationEmail</t>
+  </si>
+  <si>
+    <t>Hello,
+The automation did not find any unread emails in the last 7 days.
+If this seems unexpected, please confirm that emails are being received in the configured mailbox.
+Best regards,  
+Robot :)</t>
+  </si>
+  <si>
+    <t>BusinessExEmailSubject_NoFilteredEmails</t>
+  </si>
+  <si>
+    <t>No emails matching criteria</t>
+  </si>
+  <si>
+    <t>No unread emails found</t>
+  </si>
+  <si>
+    <t>BusinessExEmailBody_NoFilteredEmails</t>
+  </si>
+  <si>
+    <t>Hello,
+The automation did not find any emails matching the specified criteria within the last 7 days.
+If this seems unexpected, please confirm the filter phrases or email delivery.
+Best regards,
+Robot :)</t>
+  </si>
+  <si>
+    <t>BusinessExEmailSubject_NoUnreadEmails</t>
+  </si>
+  <si>
+    <t>BusinessExEmailBody_NoUnreadEmails</t>
   </si>
 </sst>
 </file>
@@ -331,10 +347,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -727,10 +739,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z30"/>
+  <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -920,74 +932,90 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="195">
       <c r="A24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="180">
       <c r="A25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="150">
       <c r="A26" s="2" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="195">
       <c r="A27" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="150">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1000,7 +1028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1058,34 +1086,34 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Refactor Dispatcher: Use CurrentMail for metadata, batch update Excel and queue with dt_NewRecords and summary
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\OneDrive - THH LLC\Documents\UiPath\T2G_EmailEnricher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1211CB50-1440-4854-8B3F-5896B67D3F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2032B6-D1C4-454A-8F38-46C1F3DC229F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -741,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>

</xml_diff>